<commit_message>
Add figures and tables with more information
</commit_message>
<xml_diff>
--- a/output/PCA/fish and scats/Nut_loadings_PCs_fish_clean_scats_nopup_coda_rob.xlsx
+++ b/output/PCA/fish and scats/Nut_loadings_PCs_fish_clean_scats_nopup_coda_rob.xlsx
@@ -14,40 +14,40 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
-    <t xml:space="preserve">Comp.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comp.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comp.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comp.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comp.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comp.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comp.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comp.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comp.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comp.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comp.11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comp.12</t>
+    <t xml:space="preserve">PC1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC12</t>
   </si>
   <si>
     <t xml:space="preserve">Nutrient</t>

</xml_diff>